<commit_message>
2023 womens WC group stage evaluated match team names
</commit_message>
<xml_diff>
--- a/src/stp/database/2023-womens-world-cup.xlsx
+++ b/src/stp/database/2023-womens-world-cup.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11214"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bruceoberg/code/soccer-tourney-poster/database/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bruceoberg/code/soccer-tourney-poster/src/stp/database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1416FFD1-E6D3-B448-99D7-121690A6A9AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE9437C8-9929-3343-A87B-BA3BFBCB5F74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4320" yWindow="3720" windowWidth="19200" windowHeight="10080" xr2:uid="{51C3DE88-701F-4CAC-8963-452186F7FFBA}"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="38400" windowHeight="19300" activeTab="1" xr2:uid="{51C3DE88-701F-4CAC-8963-452186F7FFBA}"/>
   </bookViews>
   <sheets>
     <sheet name="Tournament" sheetId="8" r:id="rId1"/>
@@ -754,7 +754,13 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="7">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
     </dxf>
@@ -809,13 +815,17 @@
     <tableColumn id="2" xr3:uid="{97337EE3-AAC3-4452-8381-1A56C6B35138}" name="home-seed"/>
     <tableColumn id="3" xr3:uid="{AEDB8750-5B25-4357-9054-E49FECC94717}" name="away-seed"/>
     <tableColumn id="4" xr3:uid="{B178F43D-E631-4314-9E59-2CDA6EDA94F1}" name="time"/>
-    <tableColumn id="5" xr3:uid="{A42548B2-C8DF-4D47-B798-8E23FCB67696}" name="venue" dataDxfId="4"/>
-    <tableColumn id="11" xr3:uid="{FC876643-4BF9-4FDA-A0ED-DF50FF384B1F}" name="home-team"/>
-    <tableColumn id="10" xr3:uid="{E5D59926-7D0A-4689-A049-F55DB0E286E9}" name="away-team"/>
-    <tableColumn id="6" xr3:uid="{A0CDBBB6-1128-45BC-8300-89FE399860C1}" name="home-score" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{95DA1082-F87D-4A64-B45A-77AEEA888386}" name="away-score" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{5865175D-2339-4B50-A707-595597D0BEF5}" name="home-tiebreaker" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{967E27DF-151D-40C4-9623-59691A5D7311}" name="away-tiebreaker" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{A42548B2-C8DF-4D47-B798-8E23FCB67696}" name="venue" dataDxfId="6"/>
+    <tableColumn id="11" xr3:uid="{FC876643-4BF9-4FDA-A0ED-DF50FF384B1F}" name="home-team" dataDxfId="1">
+      <calculatedColumnFormula>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="10" xr3:uid="{E5D59926-7D0A-4689-A049-F55DB0E286E9}" name="away-team" dataDxfId="0">
+      <calculatedColumnFormula>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{A0CDBBB6-1128-45BC-8300-89FE399860C1}" name="home-score" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{95DA1082-F87D-4A64-B45A-77AEEA888386}" name="away-score" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{5865175D-2339-4B50-A707-595597D0BEF5}" name="home-tiebreaker" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{967E27DF-151D-40C4-9623-59691A5D7311}" name="away-tiebreaker" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1150,7 +1160,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{393FFACE-29F0-47F7-B7AD-389E0D6667C5}">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -1598,8 +1608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2ABE575-0207-4299-82CD-74F27B6194DA}">
   <dimension ref="A1:K65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F50" sqref="F50:G65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1662,6 +1672,14 @@
       <c r="E2">
         <v>1</v>
       </c>
+      <c r="F2" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>NZL</v>
+      </c>
+      <c r="G2" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>NOR</v>
+      </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -1683,6 +1701,14 @@
       <c r="E3">
         <v>2</v>
       </c>
+      <c r="F3" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>AUS</v>
+      </c>
+      <c r="G3" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>IRE</v>
+      </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
@@ -1704,6 +1730,14 @@
       <c r="E4">
         <v>3</v>
       </c>
+      <c r="F4" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>PHI</v>
+      </c>
+      <c r="G4" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>SUI</v>
+      </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -1725,6 +1759,14 @@
       <c r="E5">
         <v>4</v>
       </c>
+      <c r="F5" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>NGA</v>
+      </c>
+      <c r="G5" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>CAN</v>
+      </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -1746,6 +1788,14 @@
       <c r="E6">
         <v>5</v>
       </c>
+      <c r="F6" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>ESP</v>
+      </c>
+      <c r="G6" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>CRC</v>
+      </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -1767,6 +1817,14 @@
       <c r="E7">
         <v>6</v>
       </c>
+      <c r="F7" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>ZAM</v>
+      </c>
+      <c r="G7" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>JPN</v>
+      </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -1788,6 +1846,14 @@
       <c r="E8">
         <v>7</v>
       </c>
+      <c r="F8" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>ENG</v>
+      </c>
+      <c r="G8" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>HAI</v>
+      </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -1809,6 +1875,14 @@
       <c r="E9">
         <v>8</v>
       </c>
+      <c r="F9" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>DEN</v>
+      </c>
+      <c r="G9" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>CHI</v>
+      </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -1830,6 +1904,14 @@
       <c r="E10">
         <v>1</v>
       </c>
+      <c r="F10" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>USA</v>
+      </c>
+      <c r="G10" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>VIE</v>
+      </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -1851,6 +1933,14 @@
       <c r="E11">
         <v>3</v>
       </c>
+      <c r="F11" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>NED</v>
+      </c>
+      <c r="G11" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>POR</v>
+      </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
@@ -1872,6 +1962,14 @@
       <c r="E12">
         <v>2</v>
       </c>
+      <c r="F12" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>FRA</v>
+      </c>
+      <c r="G12" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>JAM</v>
+      </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -1893,6 +1991,14 @@
       <c r="E13">
         <v>5</v>
       </c>
+      <c r="F13" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>SWE</v>
+      </c>
+      <c r="G13" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>SAF</v>
+      </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
@@ -1914,6 +2020,14 @@
       <c r="E14">
         <v>9</v>
       </c>
+      <c r="F14" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>BRA</v>
+      </c>
+      <c r="G14" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>PAN</v>
+      </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
@@ -1935,6 +2049,14 @@
       <c r="E15">
         <v>1</v>
       </c>
+      <c r="F15" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>ITA</v>
+      </c>
+      <c r="G15" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>ARG</v>
+      </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
@@ -1956,6 +2078,14 @@
       <c r="E16">
         <v>4</v>
       </c>
+      <c r="F16" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>GER</v>
+      </c>
+      <c r="G16" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>MAR</v>
+      </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
@@ -1977,6 +2107,14 @@
       <c r="E17">
         <v>2</v>
       </c>
+      <c r="F17" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>COL</v>
+      </c>
+      <c r="G17" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>KOR</v>
+      </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
@@ -1998,6 +2136,14 @@
       <c r="E18">
         <v>5</v>
       </c>
+      <c r="F18" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>NZL</v>
+      </c>
+      <c r="G18" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>PHI</v>
+      </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
@@ -2019,6 +2165,14 @@
       <c r="E19">
         <v>6</v>
       </c>
+      <c r="F19" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>SUI</v>
+      </c>
+      <c r="G19" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>NOR</v>
+      </c>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
@@ -2040,6 +2194,14 @@
       <c r="E20">
         <v>8</v>
       </c>
+      <c r="F20" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>CAN</v>
+      </c>
+      <c r="G20" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>IRE</v>
+      </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
@@ -2061,6 +2223,14 @@
       <c r="E21">
         <v>1</v>
       </c>
+      <c r="F21" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>ESP</v>
+      </c>
+      <c r="G21" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>ZAM</v>
+      </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
@@ -2082,6 +2252,14 @@
       <c r="E22">
         <v>3</v>
       </c>
+      <c r="F22" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>JPN</v>
+      </c>
+      <c r="G22" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>CRC</v>
+      </c>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
@@ -2103,6 +2281,14 @@
       <c r="E23">
         <v>7</v>
       </c>
+      <c r="F23" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>AUS</v>
+      </c>
+      <c r="G23" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>NGA</v>
+      </c>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
@@ -2124,6 +2310,14 @@
       <c r="E24">
         <v>5</v>
       </c>
+      <c r="F24" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>USA</v>
+      </c>
+      <c r="G24" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>NED</v>
+      </c>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
@@ -2145,6 +2339,14 @@
       <c r="E25">
         <v>6</v>
       </c>
+      <c r="F25" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>POR</v>
+      </c>
+      <c r="G25" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>VIE</v>
+      </c>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
@@ -2166,6 +2368,14 @@
       <c r="E26">
         <v>2</v>
       </c>
+      <c r="F26" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>ENG</v>
+      </c>
+      <c r="G26" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>DEN</v>
+      </c>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
@@ -2187,6 +2397,14 @@
       <c r="E27">
         <v>9</v>
       </c>
+      <c r="F27" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>CHI</v>
+      </c>
+      <c r="G27" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>HAI</v>
+      </c>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
@@ -2208,6 +2426,14 @@
       <c r="E28">
         <v>3</v>
       </c>
+      <c r="F28" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>ARG</v>
+      </c>
+      <c r="G28" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>SAF</v>
+      </c>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
@@ -2229,6 +2455,14 @@
       <c r="E29">
         <v>7</v>
       </c>
+      <c r="F29" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>FRA</v>
+      </c>
+      <c r="G29" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>BRA</v>
+      </c>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
@@ -2250,6 +2484,14 @@
       <c r="E30">
         <v>8</v>
       </c>
+      <c r="F30" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>PAN</v>
+      </c>
+      <c r="G30" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>JAM</v>
+      </c>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
@@ -2271,6 +2513,14 @@
       <c r="E31">
         <v>5</v>
       </c>
+      <c r="F31" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>SWE</v>
+      </c>
+      <c r="G31" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>ITA</v>
+      </c>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
@@ -2292,6 +2542,14 @@
       <c r="E32">
         <v>2</v>
       </c>
+      <c r="F32" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>GER</v>
+      </c>
+      <c r="G32" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>COL</v>
+      </c>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
@@ -2313,6 +2571,14 @@
       <c r="E33">
         <v>9</v>
       </c>
+      <c r="F33" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>KOR</v>
+      </c>
+      <c r="G33" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>MAR</v>
+      </c>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
@@ -2334,6 +2600,14 @@
       <c r="E34">
         <v>3</v>
       </c>
+      <c r="F34" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>SUI</v>
+      </c>
+      <c r="G34" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>NZL</v>
+      </c>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
@@ -2355,6 +2629,14 @@
       <c r="E35">
         <v>1</v>
       </c>
+      <c r="F35" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>NOR</v>
+      </c>
+      <c r="G35" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>PHI</v>
+      </c>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
@@ -2376,6 +2658,14 @@
       <c r="E36">
         <v>4</v>
       </c>
+      <c r="F36" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>CAN</v>
+      </c>
+      <c r="G36" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>AUS</v>
+      </c>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
@@ -2397,6 +2687,14 @@
       <c r="E37">
         <v>7</v>
       </c>
+      <c r="F37" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>IRE</v>
+      </c>
+      <c r="G37" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>NGA</v>
+      </c>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
@@ -2418,6 +2716,14 @@
       <c r="E38">
         <v>5</v>
       </c>
+      <c r="F38" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>JPN</v>
+      </c>
+      <c r="G38" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>ESP</v>
+      </c>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
@@ -2439,6 +2745,14 @@
       <c r="E39">
         <v>6</v>
       </c>
+      <c r="F39" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>CRC</v>
+      </c>
+      <c r="G39" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>ZAM</v>
+      </c>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
@@ -2460,6 +2774,14 @@
       <c r="E40">
         <v>9</v>
       </c>
+      <c r="F40" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>CHI</v>
+      </c>
+      <c r="G40" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>ENG</v>
+      </c>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
@@ -2481,6 +2803,14 @@
       <c r="E41">
         <v>8</v>
       </c>
+      <c r="F41" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>HAI</v>
+      </c>
+      <c r="G41" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>DEN</v>
+      </c>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
@@ -2502,6 +2832,14 @@
       <c r="E42">
         <v>1</v>
       </c>
+      <c r="F42" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>POR</v>
+      </c>
+      <c r="G42" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>USA</v>
+      </c>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
@@ -2523,6 +2861,14 @@
       <c r="E43">
         <v>3</v>
       </c>
+      <c r="F43" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>VIE</v>
+      </c>
+      <c r="G43" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>NED</v>
+      </c>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
@@ -2544,6 +2890,14 @@
       <c r="E44">
         <v>2</v>
       </c>
+      <c r="F44" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>PAN</v>
+      </c>
+      <c r="G44" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>FRA</v>
+      </c>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
@@ -2565,6 +2919,14 @@
       <c r="E45">
         <v>4</v>
       </c>
+      <c r="F45" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>JAM</v>
+      </c>
+      <c r="G45" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>BRA</v>
+      </c>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
@@ -2586,6 +2948,14 @@
       <c r="E46">
         <v>6</v>
       </c>
+      <c r="F46" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>ARG</v>
+      </c>
+      <c r="G46" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>SWE</v>
+      </c>
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
       <c r="J46" s="1"/>
@@ -2607,6 +2977,14 @@
       <c r="E47">
         <v>5</v>
       </c>
+      <c r="F47" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>SAF</v>
+      </c>
+      <c r="G47" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>ITA</v>
+      </c>
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
       <c r="J47" s="1"/>
@@ -2628,6 +3006,14 @@
       <c r="E48">
         <v>7</v>
       </c>
+      <c r="F48" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>KOR</v>
+      </c>
+      <c r="G48" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>GER</v>
+      </c>
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
       <c r="J48" s="1"/>
@@ -2648,6 +3034,14 @@
       </c>
       <c r="E49">
         <v>8</v>
+      </c>
+      <c r="F49" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>
+        <v>MAR</v>
+      </c>
+      <c r="G49" t="str">
+        <f>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</f>
+        <v>COL</v>
       </c>
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>

</xml_diff>

<commit_message>
correct 2023 WC match 2 venue
via claude (https://claude.ai/share/e1fc61e5-3e86-45e7-8b69-32ee1c6f221c):

According to multiple sources including FIFA and Wikipedia, this match was originally scheduled for Sydney Football Stadium (Allianz Stadium) but was relocated to Stadium Australia in January 2023 to accommodate the massive demand for tickets. Stadium Australia has a capacity of ~76,000-82,500 vs Sydney Football Stadium's ~42,000.

This was a special case - Stadium Australia was originally only scheduled to host knockout matches, but FIFA moved Australia's opening game there to enable over 100,000 fans to attend the opening day across both venues (New Zealand's match in Auckland + Australia's match in Sydney).
</commit_message>
<xml_diff>
--- a/src/stp/database/2023-womens-world-cup.xlsx
+++ b/src/stp/database/2023-womens-world-cup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bruceoberg/code/soccer-tourney-poster/src/stp/database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE9437C8-9929-3343-A87B-BA3BFBCB5F74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{244F6C3F-13C2-9648-BD40-47098C560661}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="600" windowWidth="38400" windowHeight="19300" activeTab="1" xr2:uid="{51C3DE88-701F-4CAC-8963-452186F7FFBA}"/>
   </bookViews>
@@ -756,10 +756,7 @@
   </cellStyles>
   <dxfs count="7">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="164" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
@@ -771,7 +768,10 @@
       <numFmt numFmtId="164" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
@@ -816,16 +816,16 @@
     <tableColumn id="3" xr3:uid="{AEDB8750-5B25-4357-9054-E49FECC94717}" name="away-seed"/>
     <tableColumn id="4" xr3:uid="{B178F43D-E631-4314-9E59-2CDA6EDA94F1}" name="time"/>
     <tableColumn id="5" xr3:uid="{A42548B2-C8DF-4D47-B798-8E23FCB67696}" name="venue" dataDxfId="6"/>
-    <tableColumn id="11" xr3:uid="{FC876643-4BF9-4FDA-A0ED-DF50FF384B1F}" name="home-team" dataDxfId="1">
+    <tableColumn id="11" xr3:uid="{FC876643-4BF9-4FDA-A0ED-DF50FF384B1F}" name="home-team" dataDxfId="5">
       <calculatedColumnFormula>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{E5D59926-7D0A-4689-A049-F55DB0E286E9}" name="away-team" dataDxfId="0">
+    <tableColumn id="10" xr3:uid="{E5D59926-7D0A-4689-A049-F55DB0E286E9}" name="away-team" dataDxfId="4">
       <calculatedColumnFormula>INDEX(seeds[team],MATCH(matches[[#This Row],[away-seed]],seeds[seed],0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{A0CDBBB6-1128-45BC-8300-89FE399860C1}" name="home-score" dataDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{95DA1082-F87D-4A64-B45A-77AEEA888386}" name="away-score" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{5865175D-2339-4B50-A707-595597D0BEF5}" name="home-tiebreaker" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{967E27DF-151D-40C4-9623-59691A5D7311}" name="away-tiebreaker" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{A0CDBBB6-1128-45BC-8300-89FE399860C1}" name="home-score" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{95DA1082-F87D-4A64-B45A-77AEEA888386}" name="away-score" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{5865175D-2339-4B50-A707-595597D0BEF5}" name="home-tiebreaker" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{967E27DF-151D-40C4-9623-59691A5D7311}" name="away-tiebreaker" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1164,7 +1164,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1609,7 +1609,7 @@
   <dimension ref="A1:K65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F50" sqref="F50:G65"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1699,7 +1699,7 @@
         <v>45127.416666666672</v>
       </c>
       <c r="E3">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="F3" t="str">
         <f>INDEX(seeds[team],MATCH(matches[[#This Row],[home-seed]],seeds[seed],0))</f>

</xml_diff>